<commit_message>
change related to issue with otp
</commit_message>
<xml_diff>
--- a/language_update/new_lang_variable.xlsx
+++ b/language_update/new_lang_variable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>language</t>
   </si>
@@ -54,9 +54,6 @@
     <t>child_subcat_yes_all_message</t>
   </si>
   <si>
-    <t>When delete this child sub category, it will delete all related products also. So, do you still want to delete it?</t>
-  </si>
-  <si>
     <t>child_subcat_name</t>
   </si>
   <si>
@@ -181,19 +178,47 @@
   </si>
   <si>
     <t>Size Group Option has been successfully deleted</t>
+  </si>
+  <si>
+    <t>delete_child_subcat_label</t>
+  </si>
+  <si>
+    <t>Delete Child Sub Category?</t>
+  </si>
+  <si>
+    <t>Do you want to delete this child sub category?</t>
+  </si>
+  <si>
+    <t>err_user_phone_verification</t>
+  </si>
+  <si>
+    <t>Can not verify mobile phone number, please try again</t>
+  </si>
+  <si>
+    <t>success_user_mobile_verify</t>
+  </si>
+  <si>
+    <t>User mobile verified successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,10 +241,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,9 +543,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -571,7 +599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -579,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -587,10 +615,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -598,10 +626,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -609,10 +637,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -620,10 +648,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -631,10 +659,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -642,10 +670,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -653,10 +681,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -664,10 +692,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -675,10 +703,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -686,10 +714,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -697,10 +725,10 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -708,10 +736,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -719,10 +747,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -730,10 +758,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -741,10 +769,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -752,10 +780,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -763,10 +791,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -774,10 +802,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -785,10 +813,10 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30">
@@ -796,10 +824,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -807,14 +835,47 @@
         <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change related to mange new language variable
</commit_message>
<xml_diff>
--- a/language_update/new_lang_variable.xlsx
+++ b/language_update/new_lang_variable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>language</t>
   </si>
@@ -543,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -874,6 +874,11 @@
         <v>59</v>
       </c>
     </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>